<commit_message>
AEO elec sector updates and calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/EDLE/Electricity Dispatch Logit Exponent.xlsx
+++ b/InputData/elec/EDLE/Electricity Dispatch Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\elec\EDLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\elec\EDLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B594E81E-240A-45D7-BD4A-591493174C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD24F6E-C55D-44DD-82BA-056EAC952C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -453,14 +453,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,42 +468,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -524,13 +524,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -538,12 +538,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>